<commit_message>
this commit is beta v. 2.0, pushing to client
</commit_message>
<xml_diff>
--- a/ANewDesign/testTickers.xlsx
+++ b/ANewDesign/testTickers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgb/Dropbox/Python/BETA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgb/Desktop/Stuff/Python/StockAPICaller/ANewDesign/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AA2F10-DD2A-944F-8596-70313C1B0F28}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6DD90D-CFC0-EC44-8C1C-238CC956040E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>tickers</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>AAPL</t>
+  </si>
+  <si>
+    <t>FB</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
   <dimension ref="A1:A111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -426,6 +429,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
     </row>

</xml_diff>